<commit_message>
editando labels de imagens
</commit_message>
<xml_diff>
--- a/input-image-followers-likes.xlsx
+++ b/input-image-followers-likes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>image001</t>
   </si>
@@ -111,15 +111,6 @@
   </si>
   <si>
     <t>image026</t>
-  </si>
-  <si>
-    <t>image027</t>
-  </si>
-  <si>
-    <t>image028</t>
-  </si>
-  <si>
-    <t>image029</t>
   </si>
 </sst>
 </file>
@@ -439,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +581,7 @@
         <v>2800000</v>
       </c>
       <c r="C13" s="1">
-        <v>28154</v>
+        <v>107940</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -598,10 +589,10 @@
         <v>15</v>
       </c>
       <c r="B14" s="2">
-        <v>2800000</v>
+        <v>4100000</v>
       </c>
       <c r="C14" s="1">
-        <v>68418</v>
+        <v>28825</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -609,10 +600,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="2">
-        <v>2800000</v>
+        <v>4100000</v>
       </c>
       <c r="C15" s="1">
-        <v>75475</v>
+        <v>29575</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -620,10 +611,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="2">
-        <v>2800000</v>
+        <v>4100000</v>
       </c>
       <c r="C16" s="1">
-        <v>107940</v>
+        <v>47067</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -634,7 +625,7 @@
         <v>4100000</v>
       </c>
       <c r="C17" s="1">
-        <v>28825</v>
+        <v>65789</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -642,10 +633,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="2">
-        <v>4100000</v>
+        <v>102000</v>
       </c>
       <c r="C18" s="1">
-        <v>29575</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -653,10 +644,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="2">
-        <v>4100000</v>
+        <v>102000</v>
       </c>
       <c r="C19" s="1">
-        <v>47067</v>
+        <v>3438</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -664,10 +655,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="2">
-        <v>4100000</v>
+        <v>102000</v>
       </c>
       <c r="C20" s="1">
-        <v>65789</v>
+        <v>3955</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -675,10 +666,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="2">
-        <v>102000</v>
+        <v>989000</v>
       </c>
       <c r="C21" s="1">
-        <v>2585</v>
+        <v>7593</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -686,10 +677,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="2">
-        <v>102000</v>
+        <v>989000</v>
       </c>
       <c r="C22" s="1">
-        <v>3438</v>
+        <v>8279</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -697,10 +688,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="2">
-        <v>102000</v>
+        <v>989000</v>
       </c>
       <c r="C23" s="1">
-        <v>3955</v>
+        <v>10571</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -711,7 +702,7 @@
         <v>989000</v>
       </c>
       <c r="C24" s="1">
-        <v>7593</v>
+        <v>5307</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -722,7 +713,7 @@
         <v>989000</v>
       </c>
       <c r="C25" s="1">
-        <v>8279</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -733,7 +724,7 @@
         <v>989000</v>
       </c>
       <c r="C26" s="1">
-        <v>10571</v>
+        <v>7593</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -744,39 +735,6 @@
         <v>989000</v>
       </c>
       <c r="C27" s="1">
-        <v>5307</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="2">
-        <v>989000</v>
-      </c>
-      <c r="C28" s="1">
-        <v>6500</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="2">
-        <v>989000</v>
-      </c>
-      <c r="C29" s="1">
-        <v>7593</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="2">
-        <v>989000</v>
-      </c>
-      <c r="C30" s="1">
         <v>9142</v>
       </c>
     </row>

</xml_diff>

<commit_message>
colocando as imagens no xlsx
</commit_message>
<xml_diff>
--- a/input-image-followers-likes.xlsx
+++ b/input-image-followers-likes.xlsx
@@ -1,43 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barre\Documents\projeto-multimidia\projeto-multimidia\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6555"/>
+    <workbookView windowWidth="10140" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35">
+  <si>
+    <t>imagem</t>
+  </si>
+  <si>
+    <t>followers</t>
+  </si>
+  <si>
+    <t>likes</t>
+  </si>
   <si>
     <t>image001</t>
   </si>
   <si>
-    <t>imagem</t>
-  </si>
-  <si>
-    <t>followers</t>
-  </si>
-  <si>
-    <t>likes</t>
-  </si>
-  <si>
     <t>image002</t>
   </si>
   <si>
@@ -111,30 +101,398 @@
   </si>
   <si>
     <t>image026</t>
+  </si>
+  <si>
+    <t>image028</t>
+  </si>
+  <si>
+    <t>image029</t>
+  </si>
+  <si>
+    <t>image030</t>
+  </si>
+  <si>
+    <t>image031</t>
+  </si>
+  <si>
+    <t>image032</t>
+  </si>
+  <si>
+    <t>image033</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -142,28 +500,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
+    <cellStyle name="Comma" xfId="46" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -172,7 +812,7 @@
   <a:themeElements>
     <a:clrScheme name="Escritório">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="303030"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -210,7 +850,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,7 +885,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -420,326 +1060,395 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5733333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>334937</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>20100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>334937</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>16600</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>334937</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>28300</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>4700000</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>159332</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>4700000</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>159448</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>968000</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>15018</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>1100000</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>13625</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>1600000</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>7795</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>1600000</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>19516</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>1600000</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>29892</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>1600000</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>37523</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>2800000</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>107940</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>4100000</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>28825</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>4100000</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>29575</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>4100000</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>47067</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>4100000</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <v>65789</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>102000</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <v>2585</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>102000</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <v>3438</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>102000</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="2">
         <v>3955</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>989000</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="2">
         <v>7593</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>989000</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="2">
         <v>8279</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>989000</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="2">
         <v>10571</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>989000</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="2">
         <v>5307</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>989000</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="2">
         <v>6500</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>989000</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="2">
         <v>7593</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>989000</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="2">
         <v>9142</v>
       </c>
     </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>5200000</v>
+      </c>
+      <c r="C29">
+        <v>50574</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>94900</v>
+      </c>
+      <c r="C30">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="3">
+        <v>94900</v>
+      </c>
+      <c r="C31">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="3">
+        <v>94900</v>
+      </c>
+      <c r="C32">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>478000</v>
+      </c>
+      <c r="C33">
+        <v>3854</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>478000</v>
+      </c>
+      <c r="C34">
+        <v>4695</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="3"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>